<commit_message>
Started transforming data to english
</commit_message>
<xml_diff>
--- a/Data/Characteristics.xlsx
+++ b/Data/Characteristics.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saile\OneDrive - Otto-Friedrich-Universität Bamberg\Uni\masterthesis\Thesis-Latex\graphics\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saile\OneDrive - Otto-Friedrich-Universität Bamberg\ms-framework-comparison\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6FBA766-DB8C-44AF-9BB6-5A571050F34D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C73234B5-911E-48EF-8B32-B665DF585141}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C9845FEC-008D-4837-B1FB-40E33923A0C0}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,17 +31,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="37">
   <si>
     <t>Nr.</t>
   </si>
   <si>
-    <t>Charakterisitk</t>
-  </si>
-  <si>
-    <t>Fowler &amp; Lewis</t>
-  </si>
-  <si>
     <t>The Open Group</t>
   </si>
   <si>
@@ -51,104 +45,113 @@
     <t xml:space="preserve">Dragoni et. al. </t>
   </si>
   <si>
-    <t>Service Unabhängigkeit</t>
-  </si>
-  <si>
-    <t>Größe</t>
-  </si>
-  <si>
-    <t>Kommunikation durch Interfaces</t>
-  </si>
-  <si>
-    <t>Dezentrales Datenmanagement</t>
-  </si>
-  <si>
-    <t>Design für Ausfälle</t>
-  </si>
-  <si>
-    <t>Evolutionäres Design</t>
-  </si>
-  <si>
-    <t>Automatisierung</t>
-  </si>
-  <si>
-    <t>Komponentisierung via</t>
-  </si>
-  <si>
-    <t>Services</t>
-  </si>
-  <si>
-    <t>und unintelligente Leitungen</t>
-  </si>
-  <si>
-    <t>Interne Implementierungs</t>
-  </si>
-  <si>
-    <t>details verbergen</t>
-  </si>
-  <si>
-    <t>Unabhängigkeit</t>
-  </si>
-  <si>
-    <t>Datenmanagement</t>
-  </si>
-  <si>
-    <t>Bounded Context;</t>
-  </si>
-  <si>
-    <t>Einzelne Verantwortlichkeit</t>
-  </si>
-  <si>
-    <t>Modularisierung;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Intelligente Endpunkte </t>
-  </si>
-  <si>
-    <t>Gut definiertes Interface mit</t>
-  </si>
-  <si>
-    <t>veröffentlichter Vereinbarung</t>
-  </si>
-  <si>
     <t>Highly Decoupled</t>
   </si>
   <si>
-    <t>Dezentralisierung aller Dinge</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dezentrales </t>
-  </si>
-  <si>
-    <t>Automatisierung der</t>
-  </si>
-  <si>
-    <t>Infrstruktur</t>
-  </si>
-  <si>
-    <t>Kultur der Automatisierung</t>
-  </si>
-  <si>
-    <t>einführen</t>
-  </si>
-  <si>
-    <t>Hochbelastbarkeit</t>
-  </si>
-  <si>
     <t>Evolution</t>
   </si>
   <si>
-    <t>Intelligente Endpunkte und</t>
-  </si>
-  <si>
-    <t>unintelligente Leitungen</t>
+    <t>Service Independence</t>
+  </si>
+  <si>
+    <t>Size</t>
+  </si>
+  <si>
+    <t>Well-Defined Interface</t>
+  </si>
+  <si>
+    <t>Well defined Interface with a Published Contract</t>
+  </si>
+  <si>
+    <t>Smart Endpoints and Dump Pipes</t>
+  </si>
+  <si>
+    <t>Smart endpoints and dump pipes</t>
+  </si>
+  <si>
+    <t>Decentralized Data Management</t>
+  </si>
+  <si>
+    <t>Automation</t>
+  </si>
+  <si>
+    <t>Design for failure</t>
+  </si>
+  <si>
+    <t>Design for Failure</t>
+  </si>
+  <si>
+    <t>Evolutionary Design</t>
+  </si>
+  <si>
+    <t>Componentization via Services</t>
+  </si>
+  <si>
+    <t>Infrastructure Automation</t>
+  </si>
+  <si>
+    <t>Single Responsibility</t>
+  </si>
+  <si>
+    <t>Highly Resilient</t>
+  </si>
+  <si>
+    <t>Fowler and Lewis</t>
+  </si>
+  <si>
+    <t>Characteristic</t>
+  </si>
+  <si>
+    <t>Independency</t>
+  </si>
+  <si>
+    <t>Size;
+Bounded Context;
+Modularity</t>
+  </si>
+  <si>
+    <t>Decentralize All the Things</t>
+  </si>
+  <si>
+    <t>Adopt a Culture of Automation</t>
+  </si>
+  <si>
+    <t>Highly Observable;
+Isolate Failure</t>
+  </si>
+  <si>
+    <t>Hide Internal Implementation Details</t>
+  </si>
+  <si>
+    <t>1.</t>
+  </si>
+  <si>
+    <t>2.</t>
+  </si>
+  <si>
+    <t>3.</t>
+  </si>
+  <si>
+    <t>4.</t>
+  </si>
+  <si>
+    <t>5.</t>
+  </si>
+  <si>
+    <t>6.</t>
+  </si>
+  <si>
+    <t>7.</t>
+  </si>
+  <si>
+    <t>8.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -164,8 +167,18 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="CMU Serif"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="CMU Serif"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -174,20 +187,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FFD9D9D9"/>
+        <bgColor rgb="FFBFBFBF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
   </fills>
@@ -218,13 +225,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -539,269 +548,185 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6443E267-B6CA-4468-8406-01C5015D1944}">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.44140625" customWidth="1"/>
-    <col min="2" max="2" width="28.21875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="22.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.33203125" customWidth="1"/>
-    <col min="5" max="5" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.109375" customWidth="1"/>
+    <col min="1" max="1" width="4.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.44140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="28" customWidth="1"/>
+    <col min="4" max="4" width="31.109375" customWidth="1"/>
+    <col min="5" max="5" width="17.88671875" customWidth="1"/>
+    <col min="6" max="6" width="40.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:6" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.4">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="5">
-        <v>1</v>
+    </row>
+    <row r="2" spans="1:6" ht="31.2" x14ac:dyDescent="0.4">
+      <c r="A2" s="3" t="s">
+        <v>29</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="5"/>
-      <c r="B3" s="3"/>
+    <row r="3" spans="1:6" ht="46.8" x14ac:dyDescent="0.4">
+      <c r="A3" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>7</v>
+      </c>
       <c r="C3" s="2" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="31.2" x14ac:dyDescent="0.4">
+      <c r="A4" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="5">
-        <v>2</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="31.2" x14ac:dyDescent="0.4">
+      <c r="A5" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="31.2" x14ac:dyDescent="0.4">
+      <c r="A6" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15.6" x14ac:dyDescent="0.4">
+      <c r="A7" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="5"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F5" s="2"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="5"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F6" s="2"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="5">
-        <v>3</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>8</v>
-      </c>
       <c r="C7" s="2" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="E7" s="2"/>
-      <c r="F7" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="5"/>
-      <c r="B8" s="3"/>
+      <c r="F7" s="2"/>
+    </row>
+    <row r="8" spans="1:6" ht="31.2" x14ac:dyDescent="0.4">
+      <c r="A8" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="C8" s="2" t="s">
         <v>14</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="5">
-        <v>4</v>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="15.6" x14ac:dyDescent="0.4">
+      <c r="A9" s="3" t="s">
+        <v>36</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="5"/>
-      <c r="B10" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="5">
+        <v>16</v>
+      </c>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="5"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="5">
-        <v>6</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="5"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" s="5">
-        <v>7</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" s="5">
-        <v>8</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="F16" s="2"/>
+      <c r="F9" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>